<commit_message>
Fixed wrong company ID and updated case matrix
</commit_message>
<xml_diff>
--- a/case-characterization-matrix.xlsx
+++ b/case-characterization-matrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\workspace\phd\research-microservices-interviews\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{122C230B-66E4-4B53-8596-963C9C6F5F76}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{265F7CE2-8305-4AD7-93B8-C7044EE81A4E}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14025" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="519" uniqueCount="334">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="519" uniqueCount="335">
   <si>
     <t>Company ID</t>
   </si>
@@ -1004,9 +1004,6 @@
   </si>
   <si>
     <t>~300</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1 to 30 operations / service (mean: ~5-10), 1 EAR with 20-25 jars </t>
   </si>
   <si>
     <t>RMI/RPC</t>
@@ -3366,6 +3363,12 @@
   <si>
     <t>Human resource management product from a public transport management suite (S11)</t>
   </si>
+  <si>
+    <t>on-premise, public cloud (AWS)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 to 30 operations / service (mean: 5-10), 1 EAR with 20-25 jars </t>
+  </si>
 </sst>
 </file>
 
@@ -3568,9 +3571,12 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -3579,9 +3585,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3959,13 +3962,13 @@
       </c>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="37" t="s">
+      <c r="A3" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="39" t="s">
+      <c r="B3" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="40" t="s">
+      <c r="C3" s="41" t="s">
         <v>15</v>
       </c>
       <c r="D3" s="7" t="s">
@@ -4016,13 +4019,13 @@
       </c>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="37" t="s">
+      <c r="A6" s="39" t="s">
         <v>168</v>
       </c>
-      <c r="B6" s="41" t="s">
+      <c r="B6" s="42" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="40" t="s">
+      <c r="C6" s="41" t="s">
         <v>198</v>
       </c>
       <c r="D6" s="7" t="s">
@@ -4034,7 +4037,7 @@
       <c r="F6" s="5">
         <v>20</v>
       </c>
-      <c r="G6" s="42" t="s">
+      <c r="G6" s="37" t="s">
         <v>94</v>
       </c>
     </row>
@@ -4054,13 +4057,13 @@
       <c r="G7" s="38"/>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="37" t="s">
+      <c r="A8" s="39" t="s">
         <v>232</v>
       </c>
-      <c r="B8" s="39" t="s">
+      <c r="B8" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="40" t="s">
+      <c r="C8" s="41" t="s">
         <v>237</v>
       </c>
       <c r="D8" s="7" t="s">
@@ -4117,13 +4120,13 @@
       </c>
     </row>
     <row r="11" spans="1:7">
-      <c r="A11" s="37" t="s">
+      <c r="A11" s="39" t="s">
         <v>252</v>
       </c>
-      <c r="B11" s="39" t="s">
+      <c r="B11" s="40" t="s">
         <v>253</v>
       </c>
-      <c r="C11" s="40" t="s">
+      <c r="C11" s="41" t="s">
         <v>254</v>
       </c>
       <c r="D11" s="7" t="s">
@@ -4135,7 +4138,7 @@
       <c r="F11" s="5">
         <v>9</v>
       </c>
-      <c r="G11" s="42" t="s">
+      <c r="G11" s="37" t="s">
         <v>134</v>
       </c>
     </row>
@@ -4172,17 +4175,17 @@
       </c>
     </row>
     <row r="14" spans="1:7">
-      <c r="A14" s="37" t="s">
-        <v>281</v>
-      </c>
-      <c r="B14" s="39" t="s">
-        <v>283</v>
-      </c>
-      <c r="C14" s="40" t="s">
+      <c r="A14" s="39" t="s">
+        <v>280</v>
+      </c>
+      <c r="B14" s="40" t="s">
+        <v>282</v>
+      </c>
+      <c r="C14" s="41" t="s">
         <v>237</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="E14" s="8" t="s">
         <v>154</v>
@@ -4199,10 +4202,10 @@
       <c r="B15" s="38"/>
       <c r="C15" s="38"/>
       <c r="D15" s="7" t="s">
+        <v>287</v>
+      </c>
+      <c r="E15" s="8" t="s">
         <v>288</v>
-      </c>
-      <c r="E15" s="8" t="s">
-        <v>289</v>
       </c>
       <c r="F15" s="5">
         <v>5</v>
@@ -4213,16 +4216,16 @@
     </row>
     <row r="16" spans="1:7">
       <c r="A16" s="4" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C16" s="21" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="E16" s="8" t="s">
         <v>145</v>
@@ -4236,7 +4239,7 @@
     </row>
     <row r="17" spans="1:7">
       <c r="A17" s="4" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>14</v>
@@ -4245,7 +4248,7 @@
         <v>237</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="E17" s="4" t="s">
         <v>154</v>
@@ -4259,16 +4262,16 @@
     </row>
     <row r="18" spans="1:7">
       <c r="A18" s="4" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B18" s="14" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C18" s="20" t="s">
         <v>254</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E18" s="4" t="s">
         <v>145</v>
@@ -11156,6 +11159,12 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="B3:B5"/>
+    <mergeCell ref="C3:C5"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:C7"/>
     <mergeCell ref="G6:G7"/>
     <mergeCell ref="A14:A15"/>
     <mergeCell ref="B14:B15"/>
@@ -11167,12 +11176,6 @@
     <mergeCell ref="B11:B13"/>
     <mergeCell ref="C11:C13"/>
     <mergeCell ref="G11:G12"/>
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="B3:B5"/>
-    <mergeCell ref="C3:C5"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:C7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup scale="45" orientation="landscape"/>
@@ -11184,10 +11187,10 @@
   <dimension ref="A1:M998"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -11384,7 +11387,7 @@
         <v>73</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>115</v>
+        <v>333</v>
       </c>
       <c r="F5" s="15" t="s">
         <v>117</v>
@@ -11706,7 +11709,7 @@
         <v>39</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="D13" s="14" t="s">
         <v>234</v>
@@ -11724,19 +11727,19 @@
         <v>270</v>
       </c>
       <c r="I13" s="14" t="s">
+        <v>334</v>
+      </c>
+      <c r="J13" s="12" t="s">
         <v>271</v>
-      </c>
-      <c r="J13" s="12" t="s">
-        <v>272</v>
       </c>
       <c r="K13" s="12" t="s">
         <v>267</v>
       </c>
       <c r="L13" s="12" t="s">
+        <v>272</v>
+      </c>
+      <c r="M13" s="14" t="s">
         <v>273</v>
-      </c>
-      <c r="M13" s="14" t="s">
-        <v>274</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="270">
@@ -11747,37 +11750,37 @@
         <v>39</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D14" s="14" t="s">
         <v>216</v>
       </c>
       <c r="E14" s="12" t="s">
+        <v>275</v>
+      </c>
+      <c r="F14" s="15" t="s">
         <v>276</v>
-      </c>
-      <c r="F14" s="15" t="s">
-        <v>277</v>
       </c>
       <c r="G14" s="19" t="s">
         <v>47</v>
       </c>
       <c r="H14" s="7" t="s">
+        <v>277</v>
+      </c>
+      <c r="I14" s="14" t="s">
         <v>278</v>
-      </c>
-      <c r="I14" s="14" t="s">
-        <v>279</v>
       </c>
       <c r="J14" s="12" t="s">
         <v>74</v>
       </c>
       <c r="K14" s="12" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="L14" s="12" t="s">
         <v>93</v>
       </c>
       <c r="M14" s="14" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="255">
@@ -11788,7 +11791,7 @@
         <v>68</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D15" s="14" t="s">
         <v>73</v>
@@ -11806,7 +11809,7 @@
         <v>7</v>
       </c>
       <c r="I15" s="14" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="J15" s="14" t="s">
         <v>202</v>
@@ -11818,7 +11821,7 @@
         <v>93</v>
       </c>
       <c r="M15" s="14" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="225">
@@ -11829,37 +11832,37 @@
         <v>39</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D16" s="14" t="s">
         <v>216</v>
       </c>
       <c r="E16" s="14" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="F16" s="9" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="G16" s="19" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="H16" s="7" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="I16" s="14" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="J16" s="14" t="s">
         <v>217</v>
       </c>
       <c r="K16" s="14" t="s">
+        <v>298</v>
+      </c>
+      <c r="L16" s="14" t="s">
         <v>299</v>
       </c>
-      <c r="L16" s="14" t="s">
-        <v>300</v>
-      </c>
       <c r="M16" s="14" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="17" spans="1:13">
@@ -39008,34 +39011,34 @@
         <v>6</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>305</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>306</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>307</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>308</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>309</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>310</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>311</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>312</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>313</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="L1" s="3" t="s">
         <v>314</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>315</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="409.5">
@@ -39046,7 +39049,7 @@
         <v>12</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="D2" s="14">
         <v>0</v>
@@ -39085,7 +39088,7 @@
         <v>52</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="D3" s="14">
         <v>1</v>
@@ -39124,7 +39127,7 @@
         <v>67</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="D4" s="14">
         <v>0</v>
@@ -39163,7 +39166,7 @@
         <v>81</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D5" s="14">
         <v>1</v>
@@ -39202,7 +39205,7 @@
         <v>94</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="D6" s="14">
         <v>0</v>
@@ -39241,7 +39244,7 @@
         <v>94</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="D7" s="14">
         <v>1</v>
@@ -39280,7 +39283,7 @@
         <v>103</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D8" s="14">
         <v>0</v>
@@ -39319,7 +39322,7 @@
         <v>116</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="D9" s="14">
         <v>1</v>
@@ -39358,7 +39361,7 @@
         <v>127</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="D10" s="4">
         <v>0</v>
@@ -39397,7 +39400,7 @@
         <v>134</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="D11" s="14">
         <v>0</v>
@@ -39436,7 +39439,7 @@
         <v>134</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D12" s="14">
         <v>0</v>
@@ -39475,7 +39478,7 @@
         <v>150</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D13" s="14">
         <v>0</v>
@@ -39508,13 +39511,13 @@
     </row>
     <row r="14" spans="1:12" ht="120">
       <c r="A14" s="4" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B14" s="20" t="s">
         <v>176</v>
       </c>
       <c r="C14" s="31" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="D14" s="14">
         <v>0</v>
@@ -39547,13 +39550,13 @@
     </row>
     <row r="15" spans="1:12" ht="330">
       <c r="A15" s="4" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B15" s="9" t="s">
         <v>162</v>
       </c>
       <c r="C15" s="32" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="D15" s="14">
         <v>1</v>
@@ -39586,13 +39589,13 @@
     </row>
     <row r="16" spans="1:12" ht="409.5">
       <c r="A16" s="4" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B16" s="9" t="s">
         <v>190</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D16" s="14">
         <v>0</v>
@@ -39625,13 +39628,13 @@
     </row>
     <row r="17" spans="1:12">
       <c r="A17" s="4" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B17" s="9" t="s">
         <v>197</v>
       </c>
       <c r="C17" s="33" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D17" s="14">
         <v>0</v>
@@ -39664,13 +39667,13 @@
     </row>
     <row r="18" spans="1:12" ht="409.5">
       <c r="A18" s="4" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B18" s="9" t="s">
         <v>209</v>
       </c>
       <c r="C18" s="34" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D18" s="14">
         <v>0</v>

</xml_diff>